<commit_message>
Updated graph style and hide unwanted rows in cumulative graph
</commit_message>
<xml_diff>
--- a/Project/School/Revenue Cost Model.xlsx
+++ b/Project/School/Revenue Cost Model.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Product Definition" sheetId="4" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="Cost - Benifit" sheetId="1" r:id="rId4"/>
     <sheet name="Cumulative" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -171,12 +171,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_([$INR]\ * #,##0.00_);_([$INR]\ * \(#,##0.00\);_([$INR]\ * &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -801,6 +801,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="1" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -843,12 +849,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="1" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -865,12 +865,24 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
+  <c:date1904 val="0"/>
+  <c:lang val="en-IN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1089,19 +1101,30 @@
           </c:val>
           <c:smooth val="1"/>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="77071104"/>
-        <c:axId val="77072640"/>
+        <c:smooth val="0"/>
+        <c:axId val="117355648"/>
+        <c:axId val="117357184"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="77071104"/>
+        <c:axId val="117355648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="mmm\-yy" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr/>
@@ -1113,17 +1136,18 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="77072640"/>
+        <c:crossAx val="117357184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="months"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="77072640"/>
+        <c:axId val="117357184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
@@ -1143,9 +1167,11 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr/>
@@ -1157,7 +1183,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="77071104"/>
+        <c:crossAx val="117355648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1165,6 +1191,7 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
         <a:lstStyle/>
@@ -1178,6 +1205,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -1189,12 +1217,24 @@
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
+  <c:date1904 val="0"/>
+  <c:lang val="en-IN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
+      <c:areaChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1257,46 +1297,6 @@
           <c:val>
             <c:numRef>
               <c:f>Cumulative!$B$20:$M$20</c:f>
-              <c:numCache>
-                <c:formatCode>_-* #,##0_-;\-* #,##0_-;_-* "-"_-;_-@_-</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>40000</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>40000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>40000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>80000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>104000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>156000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>156000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>156000</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>186000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>248000</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>248000</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>248000</c:v>
-                </c:pt>
-              </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
@@ -1362,46 +1362,6 @@
           <c:val>
             <c:numRef>
               <c:f>Cumulative!$B$21:$M$21</c:f>
-              <c:numCache>
-                <c:formatCode>_-* #,##0_-;\-* #,##0_-;_-* "-"_-;_-@_-</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>18200</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>18200</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>18200</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>52400</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>58640</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>59160</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>108960</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>114960</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>115260</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>189680</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>189680</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>189680</c:v>
-                </c:pt>
-              </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
@@ -1419,9 +1379,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
           <c:cat>
             <c:numRef>
               <c:f>Cumulative!$B$19:$M$19</c:f>
@@ -1512,7 +1469,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="1"/>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -1528,9 +1484,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
           <c:cat>
             <c:numRef>
               <c:f>Cumulative!$B$19:$M$19</c:f>
@@ -1621,19 +1574,28 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="1"/>
         </c:ser>
-        <c:marker val="1"/>
-        <c:axId val="77120256"/>
-        <c:axId val="77121792"/>
-      </c:lineChart>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="117769728"/>
+        <c:axId val="117771264"/>
+      </c:areaChart>
       <c:dateAx>
-        <c:axId val="77120256"/>
+        <c:axId val="117769728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="mmm\-yy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr/>
@@ -1645,20 +1607,23 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="77121792"/>
+        <c:crossAx val="117771264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="months"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="77121792"/>
+        <c:axId val="117771264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr/>
@@ -1670,14 +1635,15 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="77120256"/>
+        <c:crossAx val="117769728"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
         <a:lstStyle/>
@@ -1691,6 +1657,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -1845,6 +1812,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1879,6 +1847,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2054,17 +2023,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D15" sqref="D15"/>
+      <selection pane="bottomRight" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="22.85546875" style="1" customWidth="1"/>
@@ -2075,7 +2044,7 @@
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" ht="15.75" thickBot="1">
+    <row r="2" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D2" s="41" t="s">
         <v>28</v>
       </c>
@@ -2086,11 +2055,11 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="2:6">
-      <c r="B3" s="66" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="68" t="s">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="72" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="74" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="40" t="s">
@@ -2103,9 +2072,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="15.75" thickBot="1">
-      <c r="B4" s="67"/>
-      <c r="C4" s="69"/>
+    <row r="4" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="73"/>
+      <c r="C4" s="75"/>
       <c r="D4" s="11" t="s">
         <v>1</v>
       </c>
@@ -2116,7 +2085,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="15.75" thickBot="1">
+    <row r="5" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="7" t="s">
         <v>24</v>
       </c>
@@ -2133,7 +2102,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="6" spans="2:6">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="10" t="s">
         <v>25</v>
       </c>
@@ -2150,7 +2119,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="7" spans="2:6">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="10" t="s">
         <v>31</v>
       </c>
@@ -2167,7 +2136,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="8" spans="2:6">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="10" t="s">
         <v>36</v>
       </c>
@@ -2184,7 +2153,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="9" spans="2:6">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
         <v>26</v>
       </c>
@@ -2199,7 +2168,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="10" spans="2:6">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="10" t="s">
         <v>32</v>
       </c>
@@ -2214,7 +2183,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="11" spans="2:6">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="10" t="s">
         <v>33</v>
       </c>
@@ -2227,14 +2196,14 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="12" spans="2:6" ht="6" customHeight="1" thickBot="1">
+    <row r="12" spans="2:6" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="56"/>
       <c r="C12" s="57"/>
       <c r="D12" s="58"/>
       <c r="E12" s="58"/>
       <c r="F12" s="58"/>
     </row>
-    <row r="13" spans="2:6" ht="15.75" thickBot="1">
+    <row r="13" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="45" t="s">
         <v>4</v>
       </c>
@@ -2252,7 +2221,7 @@
         <v>31000</v>
       </c>
     </row>
-    <row r="14" spans="2:6">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="48" t="s">
         <v>2</v>
       </c>
@@ -2269,7 +2238,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="15" spans="2:6" ht="15.75" thickBot="1">
+    <row r="15" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="51" t="s">
         <v>3</v>
       </c>
@@ -2286,7 +2255,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="16" spans="2:6" ht="15.75" thickBot="1">
+    <row r="16" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="54"/>
       <c r="C16" s="55"/>
       <c r="D16" s="61">
@@ -2302,19 +2271,19 @@
         <v>69000</v>
       </c>
     </row>
-    <row r="20" spans="5:6">
+    <row r="20" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="5:6">
+    <row r="21" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="5:6">
+    <row r="22" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="5:6">
+    <row r="23" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
     </row>
@@ -2329,24 +2298,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.28515625" style="28" customWidth="1"/>
     <col min="2" max="10" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="13" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.28515625" style="80" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.28515625" style="66" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.75" thickBot="1">
+    <row r="1" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="15">
         <v>42370</v>
       </c>
@@ -2384,24 +2353,24 @@
         <v>42705</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
-      <c r="B2" s="75" t="s">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B2" s="81" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="76"/>
-      <c r="D2" s="76"/>
-      <c r="E2" s="76"/>
-      <c r="F2" s="76"/>
-      <c r="G2" s="76"/>
-      <c r="H2" s="76"/>
-      <c r="I2" s="76"/>
-      <c r="J2" s="76"/>
-      <c r="K2" s="76"/>
-      <c r="L2" s="76"/>
-      <c r="M2" s="77"/>
-    </row>
-    <row r="3" spans="1:16">
-      <c r="A3" s="78" t="s">
+      <c r="C2" s="82"/>
+      <c r="D2" s="82"/>
+      <c r="E2" s="82"/>
+      <c r="F2" s="82"/>
+      <c r="G2" s="82"/>
+      <c r="H2" s="82"/>
+      <c r="I2" s="82"/>
+      <c r="J2" s="82"/>
+      <c r="K2" s="82"/>
+      <c r="L2" s="82"/>
+      <c r="M2" s="83"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="84" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="63">
@@ -2448,8 +2417,8 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
-      <c r="A4" s="78"/>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="84"/>
       <c r="B4" s="16">
         <f>'Product Definition'!D13</f>
         <v>20000</v>
@@ -2502,8 +2471,8 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
-      <c r="A5" s="78"/>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="84"/>
       <c r="B5" s="32">
         <f>B3*B4</f>
         <v>40000</v>
@@ -2552,13 +2521,13 @@
         <f t="shared" si="0"/>
         <v>248000</v>
       </c>
-      <c r="N5" s="81">
+      <c r="N5" s="67">
         <f>SUM(B5:M5)</f>
         <v>1702000</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="1.5" hidden="1" customHeight="1">
-      <c r="A6" s="79" t="s">
+    <row r="6" spans="1:16" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="85" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="19"/>
@@ -2592,8 +2561,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="1.5" hidden="1" customHeight="1">
-      <c r="A7" s="79"/>
+    <row r="7" spans="1:16" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="85"/>
       <c r="B7" s="19"/>
       <c r="C7" s="21"/>
       <c r="D7" s="21"/>
@@ -2634,8 +2603,8 @@
         <v>38000</v>
       </c>
     </row>
-    <row r="8" spans="1:16" hidden="1">
-      <c r="A8" s="79"/>
+    <row r="8" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="85"/>
       <c r="B8" s="30">
         <f t="shared" ref="B8" si="1">B6*B7</f>
         <v>0</v>
@@ -2684,12 +2653,12 @@
         <f t="shared" ref="M8" si="12">M6*M7</f>
         <v>0</v>
       </c>
-      <c r="N8" s="82">
+      <c r="N8" s="68">
         <f>SUM(B8:M8)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="15.75" thickBot="1">
+    <row r="9" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="27"/>
       <c r="B9" s="39">
         <f t="shared" ref="B9:M9" si="13">B5+B8</f>
@@ -2739,13 +2708,13 @@
         <f t="shared" si="13"/>
         <v>248000</v>
       </c>
-      <c r="N9" s="83">
+      <c r="N9" s="69">
         <f>SUM(B9:M9)</f>
         <v>1702000</v>
       </c>
       <c r="O9" s="26"/>
     </row>
-    <row r="10" spans="1:16" ht="15.75" thickBot="1">
+    <row r="10" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="27"/>
       <c r="B10" s="17"/>
       <c r="C10" s="17"/>
@@ -2759,26 +2728,26 @@
       <c r="K10" s="17"/>
       <c r="L10" s="17"/>
       <c r="M10" s="17"/>
-      <c r="N10" s="82"/>
-    </row>
-    <row r="11" spans="1:16" ht="15.75" thickBot="1">
-      <c r="B11" s="72" t="s">
+      <c r="N10" s="68"/>
+    </row>
+    <row r="11" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="78" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="73"/>
-      <c r="D11" s="73"/>
-      <c r="E11" s="73"/>
-      <c r="F11" s="73"/>
-      <c r="G11" s="73"/>
-      <c r="H11" s="73"/>
-      <c r="I11" s="73"/>
-      <c r="J11" s="73"/>
-      <c r="K11" s="73"/>
-      <c r="L11" s="73"/>
-      <c r="M11" s="74"/>
-    </row>
-    <row r="12" spans="1:16">
-      <c r="A12" s="78" t="s">
+      <c r="C11" s="79"/>
+      <c r="D11" s="79"/>
+      <c r="E11" s="79"/>
+      <c r="F11" s="79"/>
+      <c r="G11" s="79"/>
+      <c r="H11" s="79"/>
+      <c r="I11" s="79"/>
+      <c r="J11" s="79"/>
+      <c r="K11" s="79"/>
+      <c r="L11" s="79"/>
+      <c r="M11" s="80"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="84" t="s">
         <v>7</v>
       </c>
       <c r="B12" s="63">
@@ -2818,8 +2787,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:16">
-      <c r="A13" s="78"/>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="84"/>
       <c r="B13" s="16">
         <f>B12*2000</f>
         <v>4000</v>
@@ -2872,8 +2841,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
-      <c r="A14" s="78"/>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="84"/>
       <c r="B14" s="16">
         <v>0</v>
       </c>
@@ -2911,8 +2880,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:16">
-      <c r="A15" s="78"/>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="84"/>
       <c r="B15" s="16">
         <f>B5*0.01</f>
         <v>400</v>
@@ -2965,8 +2934,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="14.25" customHeight="1">
-      <c r="A16" s="78"/>
+    <row r="16" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="84"/>
       <c r="B16" s="30">
         <f>(B12*B13)+B14+B15</f>
         <v>8400</v>
@@ -3015,13 +2984,13 @@
         <f>(M12*M13) + M14+M15</f>
         <v>130480</v>
       </c>
-      <c r="N16" s="81">
+      <c r="N16" s="67">
         <f>SUM(B16:M16) * -1</f>
         <v>-737020</v>
       </c>
     </row>
-    <row r="17" spans="1:16" ht="0.75" hidden="1" customHeight="1">
-      <c r="A17" s="78" t="s">
+    <row r="17" spans="1:16" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="84" t="s">
         <v>8</v>
       </c>
       <c r="B17" s="19"/>
@@ -3055,8 +3024,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:16" hidden="1">
-      <c r="A18" s="78"/>
+    <row r="18" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="84"/>
       <c r="B18" s="32"/>
       <c r="C18" s="33"/>
       <c r="D18" s="33"/>
@@ -3088,8 +3057,8 @@
         <v>25000</v>
       </c>
     </row>
-    <row r="19" spans="1:16" ht="0.75" hidden="1" customHeight="1">
-      <c r="A19" s="78"/>
+    <row r="19" spans="1:16" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="84"/>
       <c r="B19" s="30">
         <f t="shared" ref="B19" si="17">B17*B18</f>
         <v>0</v>
@@ -3138,13 +3107,13 @@
         <f t="shared" ref="M19" si="28">M17*M18</f>
         <v>0</v>
       </c>
-      <c r="N19" s="81">
+      <c r="N19" s="67">
         <f>SUM(B19:M19)*-1</f>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:16">
-      <c r="A20" s="70" t="s">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A20" s="76" t="s">
         <v>17</v>
       </c>
       <c r="B20" s="19"/>
@@ -3163,8 +3132,8 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:16">
-      <c r="A21" s="70"/>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A21" s="76"/>
       <c r="B21" s="35"/>
       <c r="C21" s="36"/>
       <c r="D21" s="36"/>
@@ -3184,8 +3153,8 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="22" spans="1:16">
-      <c r="A22" s="70"/>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A22" s="76"/>
       <c r="B22" s="32">
         <f t="shared" ref="B22" si="29">B20*B21</f>
         <v>0</v>
@@ -3234,13 +3203,13 @@
         <f t="shared" ref="M22" si="40">M20*M21</f>
         <v>0</v>
       </c>
-      <c r="N22" s="81">
+      <c r="N22" s="67">
         <f>SUM(F22:M22)*-1</f>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:16">
-      <c r="A23" s="70" t="s">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A23" s="76" t="s">
         <v>12</v>
       </c>
       <c r="B23" s="19"/>
@@ -3275,8 +3244,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:16">
-      <c r="A24" s="70"/>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A24" s="76"/>
       <c r="B24" s="35"/>
       <c r="C24" s="36"/>
       <c r="D24" s="36"/>
@@ -3306,8 +3275,8 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="25" spans="1:16">
-      <c r="A25" s="70"/>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A25" s="76"/>
       <c r="B25" s="32">
         <f t="shared" ref="B25:C25" si="41">B23*B24</f>
         <v>0</v>
@@ -3356,13 +3325,13 @@
         <f t="shared" ref="M25" si="51">M23*M24</f>
         <v>20000</v>
       </c>
-      <c r="N25" s="81">
+      <c r="N25" s="67">
         <f>SUM(F25:M25)*-1</f>
         <v>-102000</v>
       </c>
     </row>
-    <row r="26" spans="1:16">
-      <c r="A26" s="71" t="s">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A26" s="77" t="s">
         <v>13</v>
       </c>
       <c r="B26" s="19"/>
@@ -3378,8 +3347,8 @@
       <c r="L26" s="21"/>
       <c r="M26" s="22"/>
     </row>
-    <row r="27" spans="1:16">
-      <c r="A27" s="71"/>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A27" s="77"/>
       <c r="B27" s="35"/>
       <c r="C27" s="36"/>
       <c r="D27" s="36"/>
@@ -3402,8 +3371,8 @@
         <v>14</v>
       </c>
     </row>
-    <row r="28" spans="1:16">
-      <c r="A28" s="71"/>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A28" s="77"/>
       <c r="B28" s="30">
         <f t="shared" ref="B28" si="52">B26*B27</f>
         <v>0</v>
@@ -3452,12 +3421,12 @@
         <f t="shared" ref="M28" si="62">M26*M27</f>
         <v>0</v>
       </c>
-      <c r="N28" s="81">
+      <c r="N28" s="67">
         <f>SUM(K28:M28)*-1</f>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:16">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="28" t="s">
         <v>16</v>
       </c>
@@ -3509,9 +3478,9 @@
         <f>600*4*M12</f>
         <v>19200</v>
       </c>
-      <c r="N29" s="81"/>
-    </row>
-    <row r="30" spans="1:16">
+      <c r="N29" s="67"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="28" t="s">
         <v>18</v>
       </c>
@@ -3527,9 +3496,9 @@
       <c r="K30" s="21"/>
       <c r="L30" s="21"/>
       <c r="M30" s="22"/>
-      <c r="N30" s="81"/>
-    </row>
-    <row r="31" spans="1:16">
+      <c r="N30" s="67"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="28" t="s">
         <v>19</v>
       </c>
@@ -3545,9 +3514,9 @@
       <c r="K31" s="21"/>
       <c r="L31" s="21"/>
       <c r="M31" s="22"/>
-      <c r="N31" s="81"/>
-    </row>
-    <row r="32" spans="1:16">
+      <c r="N31" s="67"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="28" t="s">
         <v>15</v>
       </c>
@@ -3587,9 +3556,9 @@
       <c r="M32" s="34">
         <v>20000</v>
       </c>
-      <c r="N32" s="81"/>
-    </row>
-    <row r="33" spans="2:15" ht="15.75" thickBot="1">
+      <c r="N32" s="67"/>
+    </row>
+    <row r="33" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="16">
         <f>SUM(B29:B32)</f>
         <v>9800</v>
@@ -3638,12 +3607,12 @@
         <f t="shared" si="64"/>
         <v>39200</v>
       </c>
-      <c r="N33" s="81">
+      <c r="N33" s="67">
         <f>SUM(B33:M33)*-1</f>
         <v>-294000</v>
       </c>
     </row>
-    <row r="34" spans="2:15" ht="15.75" thickBot="1">
+    <row r="34" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="23">
         <f>B16+B19+B22+B25+B28+B33</f>
         <v>18200</v>
@@ -3692,13 +3661,13 @@
         <f t="shared" si="65"/>
         <v>189680</v>
       </c>
-      <c r="N34" s="84">
+      <c r="N34" s="70">
         <f>SUM(B34:M34)</f>
         <v>1133020</v>
       </c>
       <c r="O34" s="14"/>
     </row>
-    <row r="35" spans="2:15" ht="15.75" thickBot="1">
+    <row r="35" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B35" s="23">
         <f t="shared" ref="B35:M35" si="66">B9-B34</f>
         <v>21800</v>
@@ -3747,7 +3716,7 @@
         <f t="shared" si="66"/>
         <v>58320</v>
       </c>
-      <c r="N35" s="85">
+      <c r="N35" s="71">
         <f>SUM(B35:M35)</f>
         <v>568980</v>
       </c>
@@ -3772,32 +3741,30 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A18:O20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20:M20"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="13" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="14" max="15" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="18" spans="1:15">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B18" s="12">
         <v>42370</v>
       </c>
@@ -3835,7 +3802,7 @@
         <v>42705</v>
       </c>
     </row>
-    <row r="19" spans="1:15">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>5</v>
       </c>
@@ -3890,7 +3857,7 @@
       <c r="N19" s="13"/>
       <c r="O19" s="13"/>
     </row>
-    <row r="20" spans="1:15">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>6</v>
       </c>
@@ -3952,12 +3919,12 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A19:O24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="13" width="10.5703125" bestFit="1" customWidth="1"/>
@@ -3965,7 +3932,7 @@
     <col min="15" max="15" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="19" spans="1:15">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B19" s="12">
         <v>42370</v>
       </c>
@@ -4003,7 +3970,7 @@
         <v>42705</v>
       </c>
     </row>
-    <row r="20" spans="1:15">
+    <row r="20" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>5</v>
       </c>
@@ -4058,7 +4025,7 @@
       <c r="N20" s="13"/>
       <c r="O20" s="13"/>
     </row>
-    <row r="21" spans="1:15">
+    <row r="21" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>6</v>
       </c>
@@ -4113,7 +4080,7 @@
       <c r="N21" s="13"/>
       <c r="O21" s="13"/>
     </row>
-    <row r="22" spans="1:15">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>5</v>
       </c>
@@ -4166,7 +4133,7 @@
         <v>1702000</v>
       </c>
     </row>
-    <row r="23" spans="1:15">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>6</v>
       </c>
@@ -4219,7 +4186,7 @@
         <v>1133020</v>
       </c>
     </row>
-    <row r="24" spans="1:15">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B24" s="13"/>
       <c r="C24" s="13"/>
       <c r="D24" s="13"/>

</xml_diff>